<commit_message>
modified code and structure of code
</commit_message>
<xml_diff>
--- a/questions/recommended1.xlsx
+++ b/questions/recommended1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -891,7 +891,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>July</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -904,26 +904,26 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>STL526_539_537 | Quinta da Regaleira &amp; Moorish Castle Tickets with 3 Audios</t>
+          <t>STL526_539_537 | Sintra: Moorish Castle &amp; Quinta da Regaleira e-Tickets</t>
         </is>
       </c>
       <c r="B12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
         <v>4</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
         <v>8</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
       <c r="G12" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>June</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -945,26 +945,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>STL526_539_537 | Sintra: Moorish Castle &amp; Quinta da Regaleira e-Tickets</t>
+          <t>STL526_539_537 | Quinta da Regaleira &amp; Moorish Castle Tickets with 3 Audios</t>
         </is>
       </c>
       <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="n">
         <v>8</v>
       </c>
-      <c r="C13" t="n">
-        <v>4</v>
-      </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -973,7 +973,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>August</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -1273,26 +1273,26 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>STL526_539_537 | Sintra: Moorish Castle &amp; Quinta da Regaleira e-Tickets</t>
+          <t>STL526_539_537 | Quinta da Regaleira &amp; Moorish Castle Tickets with 3 Audios</t>
         </is>
       </c>
       <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
         <v>8</v>
       </c>
-      <c r="C21" t="n">
-        <v>4</v>
-      </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>June</t>
         </is>
       </c>
       <c r="J21" t="n">
@@ -1314,26 +1314,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>STL526_539_537 | Quinta da Regaleira &amp; Moorish Castle Tickets with 3 Audios</t>
+          <t>STL526_539_537 | Sintra: Moorish Castle &amp; Quinta da Regaleira e-Tickets</t>
         </is>
       </c>
       <c r="B22" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" t="n">
         <v>4</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
         <v>8</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
       <c r="G22" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>August</t>
         </is>
       </c>
       <c r="J22" t="n">
@@ -1478,14 +1478,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>STL539_537 | Sintra: Quinta da Regaleira Ticket &amp; Sintra Smartphone Tour</t>
+          <t>STL539_537 | Quinta da Regaleira Ticket with Audio Guide &amp; Sintra Tour</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>May</t>
         </is>
       </c>
       <c r="J26" t="n">
@@ -1519,14 +1519,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>STL539_537 | Quinta da Regaleira Ticket with Audio Guide &amp; Sintra Tour</t>
+          <t>STL539_537 | Sintra: Quinta da Regaleira Ticket &amp; Sintra Smartphone Tour</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1538,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>August</t>
         </is>
       </c>
       <c r="J27" t="n">
@@ -1560,14 +1560,14 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>STL539_537 | Sintra: Quinta da Regaleira e-Ticket &amp; Sintra City Audios</t>
+          <t>STL539_537 | Sintra: Quinta da Regaleira Ticket &amp; Sintra Smartphone Tour</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -1576,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>June</t>
         </is>
       </c>
       <c r="J28" t="n">
@@ -1601,14 +1601,14 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>STL539_537 | Sintra: Quinta da Regaleira Ticket &amp; Sintra Smartphone Tour</t>
+          <t>STL539_537 | Sintra: Quinta da Regaleira e-Ticket &amp; Sintra City Audios</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1617,10 +1617,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G29" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>July</t>
         </is>
       </c>
       <c r="J29" t="n">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>March</t>
         </is>
       </c>
       <c r="J33" t="n">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>January</t>
         </is>
       </c>
       <c r="J34" t="n">
@@ -1847,26 +1847,26 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TO240_181_51_278 | Acropolis, Acropolis Museum &amp; 6 Archaeological Sites Tickets</t>
+          <t>TO240_181_51_459 | Acropolis &amp; 6 Archaeological Sites Combo Ticket</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C35" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>February</t>
         </is>
       </c>
       <c r="J35" t="n">
@@ -1888,27 +1888,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TO240_181_51_459 | Acropolis &amp; 6 Archaeological Sites Combo Ticket</t>
+          <t>TO240_181_51_278 | Acropolis, Acropolis Museum &amp; 6 Archaeological Sites Tickets</t>
         </is>
       </c>
       <c r="B36" t="n">
+        <v>12</v>
+      </c>
+      <c r="C36" t="n">
+        <v>6</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
         <v>18</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>18</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>36</v>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
           <t>Greece</t>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>March</t>
         </is>
       </c>
       <c r="J36" t="n">
@@ -1929,27 +1929,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TO240_181_51_459 | Acropolis &amp; 6 Archaeological Sites Combo Ticket</t>
+          <t>TO240_181_51_278 | Acropolis, Acropolis Museum &amp; 6 Archaeological Sites Tickets</t>
         </is>
       </c>
       <c r="B37" t="n">
+        <v>12</v>
+      </c>
+      <c r="C37" t="n">
+        <v>6</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
         <v>18</v>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>18</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>36</v>
-      </c>
       <c r="H37" t="inlineStr">
         <is>
           <t>Greece</t>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>June</t>
         </is>
       </c>
       <c r="J37" t="n">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>August</t>
         </is>
       </c>
       <c r="J38" t="n">
@@ -2011,26 +2011,26 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TO240_181_51_278 | Acropolis, Acropolis Museum &amp; 6 Archaeological Sites Tickets</t>
+          <t>TO240_181_51_459 | Acropolis &amp; 6 Archaeological Sites Combo Ticket</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C39" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>May</t>
         </is>
       </c>
       <c r="J39" t="n">
@@ -2285,14 +2285,14 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>June</t>
         </is>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46">
@@ -2326,14 +2326,14 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>May</t>
         </is>
       </c>
       <c r="J46" t="n">
         <v>0</v>
       </c>
       <c r="K46" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
@@ -2367,14 +2367,14 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>July</t>
         </is>
       </c>
       <c r="J47" t="n">
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">

</xml_diff>